<commit_message>
configured alignment for poster and demo
</commit_message>
<xml_diff>
--- a/src/main/resources/data/calendars_iswc2015/sessions.xlsx
+++ b/src/main/resources/data/calendars_iswc2015/sessions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="34880" yWindow="1500" windowWidth="25600" windowHeight="16580" tabRatio="500"/>
+    <workbookView xWindow="38740" yWindow="2260" windowWidth="25600" windowHeight="16580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="62">
   <si>
     <t>Opening Ceremony</t>
   </si>
@@ -75,9 +75,6 @@
     <t>Vision Bar and Bucks</t>
   </si>
   <si>
-    <t>13.10.2015</t>
-  </si>
-  <si>
     <t>Keynote: Andrew McCallum</t>
   </si>
   <si>
@@ -117,9 +114,6 @@
     <t>Dinner and Entertainment</t>
   </si>
   <si>
-    <t>14.10.2015</t>
-  </si>
-  <si>
     <t>Keynote: Ian Horrocks</t>
   </si>
   <si>
@@ -141,9 +135,6 @@
     <t>Closing and Awards</t>
   </si>
   <si>
-    <t>15.10.2015</t>
-  </si>
-  <si>
     <t># Date</t>
   </si>
   <si>
@@ -199,6 +190,21 @@
   </si>
   <si>
     <t>Opening</t>
+  </si>
+  <si>
+    <t>13.10.15</t>
+  </si>
+  <si>
+    <t>14.10.15</t>
+  </si>
+  <si>
+    <t>15.10.15</t>
+  </si>
+  <si>
+    <t>Posters</t>
+  </si>
+  <si>
+    <t>Demos</t>
   </si>
 </sst>
 </file>
@@ -254,8 +260,54 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="73">
+  <cellStyleXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -335,7 +387,7 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="73">
+  <cellStyles count="119">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -372,6 +424,29 @@
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -408,6 +483,29 @@
     <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -737,10 +835,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -757,33 +855,33 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" t="s">
         <v>41</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>42</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>43</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>44</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>45</v>
-      </c>
-      <c r="F1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="B2" s="2">
         <v>0.35416666666666669</v>
@@ -801,7 +899,7 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="H2" t="s">
         <v>0</v>
@@ -809,7 +907,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="B3" s="2">
         <v>0.375</v>
@@ -827,15 +925,15 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="B4" s="2">
         <v>0.42708333333333331</v>
@@ -853,7 +951,7 @@
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H4" t="s">
         <v>3</v>
@@ -861,7 +959,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="B5" s="2">
         <v>0.45833333333333331</v>
@@ -879,7 +977,7 @@
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H5" t="s">
         <v>4</v>
@@ -887,10 +985,14 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
+        <v>57</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.52083333333333337</v>
+      </c>
       <c r="D6" t="s">
         <v>5</v>
       </c>
@@ -901,7 +1003,7 @@
         <v>6</v>
       </c>
       <c r="G6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H6" t="s">
         <v>5</v>
@@ -909,10 +1011,14 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+        <v>57</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.52083333333333337</v>
+      </c>
       <c r="D7" t="s">
         <v>7</v>
       </c>
@@ -923,7 +1029,7 @@
         <v>8</v>
       </c>
       <c r="G7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H7" t="s">
         <v>7</v>
@@ -931,7 +1037,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="B8" s="2">
         <v>0.52083333333333337</v>
@@ -949,15 +1055,15 @@
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="B9" s="2">
         <v>0.58333333333333337</v>
@@ -975,7 +1081,7 @@
         <v>8</v>
       </c>
       <c r="G9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H9" t="s">
         <v>10</v>
@@ -983,10 +1089,14 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
+        <v>57</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.63888888888888895</v>
+      </c>
       <c r="D10" t="s">
         <v>11</v>
       </c>
@@ -997,7 +1107,7 @@
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H10" t="s">
         <v>11</v>
@@ -1005,10 +1115,14 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
+        <v>57</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.63888888888888895</v>
+      </c>
       <c r="D11" t="s">
         <v>12</v>
       </c>
@@ -1019,7 +1133,7 @@
         <v>6</v>
       </c>
       <c r="G11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H11" t="s">
         <v>12</v>
@@ -1027,7 +1141,7 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="B12" s="2">
         <v>0.63888888888888895</v>
@@ -1045,7 +1159,7 @@
         <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H12" t="s">
         <v>3</v>
@@ -1053,7 +1167,7 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="B13" s="2">
         <v>0.66666666666666663</v>
@@ -1071,7 +1185,7 @@
         <v>6</v>
       </c>
       <c r="G13" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H13" t="s">
         <v>13</v>
@@ -1079,10 +1193,14 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+        <v>57</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.72222222222222221</v>
+      </c>
       <c r="D14" t="s">
         <v>14</v>
       </c>
@@ -1093,7 +1211,7 @@
         <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H14" t="s">
         <v>14</v>
@@ -1101,10 +1219,14 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
+        <v>57</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.72222222222222221</v>
+      </c>
       <c r="D15" t="s">
         <v>15</v>
       </c>
@@ -1115,7 +1237,7 @@
         <v>8</v>
       </c>
       <c r="G15" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H15" t="s">
         <v>15</v>
@@ -1123,7 +1245,7 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="B16" s="2">
         <v>0.77083333333333337</v>
@@ -1141,7 +1263,7 @@
         <v>17</v>
       </c>
       <c r="G16" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H16" t="s">
         <v>16</v>
@@ -1149,616 +1271,704 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="B17" s="2">
-        <v>0.375</v>
+        <v>0.77083333333333337</v>
       </c>
       <c r="C17" s="2">
-        <v>0.42708333333333331</v>
+        <v>0.875</v>
       </c>
       <c r="D17" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
       <c r="E17" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F17" t="s">
-        <v>1</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>49</v>
+        <v>17</v>
+      </c>
+      <c r="G17" t="s">
+        <v>55</v>
+      </c>
+      <c r="H17" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="B18" s="2">
-        <v>0.42708333333333331</v>
+        <v>0.77083333333333337</v>
       </c>
       <c r="C18" s="2">
-        <v>0.45833333333333331</v>
+        <v>0.875</v>
       </c>
       <c r="D18" t="s">
-        <v>3</v>
+        <v>61</v>
       </c>
       <c r="E18" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="F18" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="G18" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="H18" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="B19" s="2">
-        <v>0.45833333333333331</v>
+        <v>0.375</v>
       </c>
       <c r="C19" s="2">
-        <v>0.52083333333333337</v>
+        <v>0.42708333333333331</v>
       </c>
       <c r="D19" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E19" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F19" t="s">
         <v>1</v>
       </c>
-      <c r="G19" t="s">
-        <v>52</v>
-      </c>
-      <c r="H19" t="s">
-        <v>20</v>
+      <c r="G19" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
+        <v>58</v>
+      </c>
+      <c r="B20" s="2">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0.45833333333333331</v>
+      </c>
       <c r="D20" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="E20" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="F20" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G20" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H20" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
+        <v>58</v>
+      </c>
+      <c r="B21" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0.52083333333333337</v>
+      </c>
       <c r="D21" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E21" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F21" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G21" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H21" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="1" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="B22" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C22" s="2">
         <v>0.52083333333333337</v>
       </c>
-      <c r="C22" s="2">
-        <v>0.58333333333333337</v>
-      </c>
       <c r="D22" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E22" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F22" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="G22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H22" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+        <v>58</v>
+      </c>
+      <c r="B23" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0.52083333333333337</v>
+      </c>
       <c r="D23" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="E23" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="F23" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H23" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="1" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="B24" s="2">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="C24" s="2">
         <v>0.58333333333333337</v>
       </c>
-      <c r="C24" s="2">
-        <v>0.63888888888888895</v>
-      </c>
       <c r="D24" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E24" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F24" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="G24" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="H24" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
+        <v>58</v>
+      </c>
+      <c r="B25" s="2">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="D25" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="E25" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="F25" t="s">
         <v>1</v>
       </c>
       <c r="G25" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H25" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
+        <v>58</v>
+      </c>
+      <c r="B26" s="2">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0.63888888888888895</v>
+      </c>
       <c r="D26" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E26" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F26" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H26" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="1" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="B27" s="2">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C27" s="2">
         <v>0.63888888888888895</v>
       </c>
-      <c r="C27" s="2">
-        <v>0.66666666666666663</v>
-      </c>
       <c r="D27" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="E27" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="F27" t="s">
         <v>1</v>
       </c>
       <c r="G27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H27" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="1" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="B28" s="2">
-        <v>0.66666666666666663</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="C28" s="2">
-        <v>0.70833333333333337</v>
+        <v>0.63888888888888895</v>
       </c>
       <c r="D28" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E28" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F28" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G28" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H28" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
+        <v>58</v>
+      </c>
+      <c r="B29" s="2">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="C29" s="2">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="D29" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="E29" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="F29" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G29" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="H29" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="1" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="B30" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C30" s="2">
         <v>0.70833333333333337</v>
       </c>
-      <c r="C30" s="2">
-        <v>0.75</v>
-      </c>
       <c r="D30" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E30" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F30" t="s">
         <v>8</v>
       </c>
       <c r="G30" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="H30" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="1" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="B31" s="2">
-        <v>0.79166666666666663</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="C31" s="2">
-        <v>0.95833333333333337</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="D31" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E31" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F31" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G31" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H31" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="1" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="B32" s="2">
-        <v>0.375</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="C32" s="2">
-        <v>0.42708333333333331</v>
+        <v>0.75</v>
       </c>
       <c r="D32" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E32" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F32" t="s">
-        <v>1</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H32" s="3" t="s">
-        <v>49</v>
+        <v>8</v>
+      </c>
+      <c r="G32" t="s">
+        <v>54</v>
+      </c>
+      <c r="H32" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="1" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="B33" s="2">
-        <v>0.42708333333333331</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="C33" s="2">
-        <v>0.45833333333333331</v>
+        <v>0.95833333333333337</v>
       </c>
       <c r="D33" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="E33" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="F33" t="s">
         <v>1</v>
       </c>
       <c r="G33" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H33" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="1" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="B34" s="2">
-        <v>0.45833333333333331</v>
+        <v>0.375</v>
       </c>
       <c r="C34" s="2">
-        <v>0.52083333333333337</v>
+        <v>0.42708333333333331</v>
       </c>
       <c r="D34" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E34" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F34" t="s">
         <v>1</v>
       </c>
-      <c r="G34" t="s">
-        <v>52</v>
-      </c>
-      <c r="H34" t="s">
-        <v>34</v>
+      <c r="G34" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
+        <v>59</v>
+      </c>
+      <c r="B35" s="2">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="C35" s="2">
+        <v>0.45833333333333331</v>
+      </c>
       <c r="D35" t="s">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="E35" t="s">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="F35" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G35" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H35" t="s">
-        <v>35</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
+        <v>59</v>
+      </c>
+      <c r="B36" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C36" s="2">
+        <v>0.52083333333333337</v>
+      </c>
       <c r="D36" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E36" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F36" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G36" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H36" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="1" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="B37" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C37" s="2">
         <v>0.52083333333333337</v>
       </c>
-      <c r="C37" s="2">
-        <v>0.58333333333333337</v>
-      </c>
       <c r="D37" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="E37" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="F37" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G37" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H37" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="1" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="B38" s="2">
-        <v>0.58333333333333337</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="C38" s="2">
-        <v>0.63888888888888895</v>
+        <v>0.52083333333333337</v>
       </c>
       <c r="D38" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E38" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F38" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G38" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H38" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
+        <v>59</v>
+      </c>
+      <c r="B39" s="2">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="C39" s="2">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="D39" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="E39" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="F39" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G39" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H39" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="1" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="B40" s="2">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C40" s="2">
         <v>0.63888888888888895</v>
       </c>
-      <c r="C40" s="2">
-        <v>0.66666666666666663</v>
-      </c>
       <c r="D40" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="E40" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="F40" t="s">
         <v>1</v>
       </c>
       <c r="G40" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H40" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="1" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="B41" s="2">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C41" s="2">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="D41" t="s">
+        <v>36</v>
+      </c>
+      <c r="E41" t="s">
+        <v>36</v>
+      </c>
+      <c r="F41" t="s">
+        <v>8</v>
+      </c>
+      <c r="G41" t="s">
+        <v>49</v>
+      </c>
+      <c r="H41" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B42" s="2">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="C42" s="2">
         <v>0.66666666666666663</v>
       </c>
-      <c r="C41" s="2">
+      <c r="D42" t="s">
+        <v>3</v>
+      </c>
+      <c r="E42" t="s">
+        <v>3</v>
+      </c>
+      <c r="F42" t="s">
+        <v>1</v>
+      </c>
+      <c r="G42" t="s">
+        <v>47</v>
+      </c>
+      <c r="H42" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B43" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C43" s="2">
         <v>0.70833333333333337</v>
       </c>
-      <c r="D41" t="s">
-        <v>39</v>
-      </c>
-      <c r="E41" t="s">
-        <v>39</v>
-      </c>
-      <c r="F41" t="s">
-        <v>1</v>
-      </c>
-      <c r="G41" t="s">
-        <v>56</v>
-      </c>
-      <c r="H41" t="s">
-        <v>39</v>
+      <c r="D43" t="s">
+        <v>37</v>
+      </c>
+      <c r="E43" t="s">
+        <v>37</v>
+      </c>
+      <c r="F43" t="s">
+        <v>1</v>
+      </c>
+      <c r="G43" t="s">
+        <v>53</v>
+      </c>
+      <c r="H43" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>